<commit_message>
CU Consultar grupos y rentas.
Parte del CU Consultar grupos y rentas, interfaz y carga de grupos, y se
actualizan plantillas de tareas y casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0696B08-89BD-44D6-ACEF-865B77041AE7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C972C429-FCA7-472E-90DF-1592438773DB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,12 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -438,6 +432,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,7 +749,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,84 +824,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="18"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="18"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="18"/>
+      <c r="O4" s="25"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="18"/>
+      <c r="R4" s="25"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="17" t="s">
+      <c r="T4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="18"/>
+      <c r="U4" s="25"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="17" t="s">
+      <c r="W4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="18"/>
+      <c r="X4" s="25"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="17" t="s">
+      <c r="Z4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="18"/>
+      <c r="AA4" s="25"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="17" t="s">
+      <c r="AC4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="18"/>
+      <c r="AD4" s="25"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="17" t="s">
+      <c r="AF4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="18"/>
+      <c r="AG4" s="25"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="17" t="s">
+      <c r="AI4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="18"/>
+      <c r="AJ4" s="25"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="17" t="s">
+      <c r="AL4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="18"/>
+      <c r="AM4" s="25"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="17" t="s">
+      <c r="AO4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="18"/>
+      <c r="AP4" s="25"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="17" t="s">
+      <c r="AR4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="18"/>
+      <c r="AS4" s="25"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="17" t="s">
+      <c r="AU4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="18"/>
+      <c r="AV4" s="25"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="17" t="s">
+      <c r="AX4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="18"/>
-      <c r="AZ4" s="17" t="s">
+      <c r="AY4" s="25"/>
+      <c r="AZ4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="18"/>
+      <c r="BA4" s="25"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1036,10 +1036,10 @@
     <row r="6" spans="2:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1149,10 +1149,10 @@
     <row r="7" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="19" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1161,111 +1161,113 @@
       <c r="G7" s="5">
         <v>4</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
       <c r="I7" s="8">
         <f t="shared" ref="I7:I16" si="16">G7-H7</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1375,10 +1377,10 @@
     <row r="9" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1488,10 +1490,10 @@
     <row r="10" spans="2:53" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1601,10 +1603,10 @@
     <row r="11" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1714,7 +1716,7 @@
     <row r="12" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="19"/>
+      <c r="D12" s="17"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="8"/>
@@ -2551,6 +2553,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2562,11 +2569,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementacion parcial del caso de uso generar recibo de pago
Se implementa parcialmente el caso de uso generar recibo de pago y actualizan plantillas de la iteracion
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C972C429-FCA7-472E-90DF-1592438773DB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A5ED5A9-80D2-4345-8FC7-D05EEF1BE613}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -749,7 +749,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,102 +1048,104 @@
       <c r="G6" s="5">
         <v>4</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="8">
+        <v>2</v>
+      </c>
       <c r="I6" s="8">
         <f>G6-H6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
         <f t="shared" ref="L6:L16" si="0">I6-K6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O16" si="1">L6-N6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R16" si="2">O6-Q6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U16" si="3">R6-T6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X16" si="4">U6-W6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA16" si="5">X6-Z6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD16" si="6">AA6-AC6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG16" si="7">AD6-AF6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ16" si="8">AG6-AI6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM16" si="9">AJ6-AL6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP16" si="10">AM6-AO6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS16" si="11">AP6-AR6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV16" si="12">AS6-AU6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY16" si="13">AV6-AX6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA16" si="15">G6-AZ6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2553,11 +2555,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2569,6 +2566,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alumnos por grupo (consultar grupos y rentas)
Se implementa la vista de alumnos por grupo para el CU Consultar grupos
y rentas, se reemplaza el establecimiento de color de fondo del panel
alumno del controlador del catálogo al panel alumno, se carga la imagen
del profesor en la ventana modificar cuenta y se actualizan plantillas
de lista de tareas y casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A5ED5A9-80D2-4345-8FC7-D05EEF1BE613}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFFFFCA-86CA-4343-9F99-A3538D2D454B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>Columna</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Víctor</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1046,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1158,7 +1161,7 @@
         <v>48</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G7" s="5">
         <v>4</v>
@@ -1171,96 +1174,98 @@
         <v>2</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2555,6 +2560,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2566,11 +2576,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementacion parcial de generar recibo de pago de alumno.
Se implementa generar recibo de pago de alumno y se actualizan plantillas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AAFB6E-0420-48AF-A2B8-7F706E1F5065}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F88AE7D5-81E9-486D-BA14-05C588728F8D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,96 +1062,98 @@
         <v>2</v>
       </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="8">
+        <v>1</v>
+      </c>
       <c r="L6" s="8">
         <f t="shared" ref="L6:L16" si="0">I6-K6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O16" si="1">L6-N6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R16" si="2">O6-Q6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U16" si="3">R6-T6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X16" si="4">U6-W6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA16" si="5">X6-Z6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD16" si="6">AA6-AC6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG16" si="7">AD6-AF6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ16" si="8">AG6-AI6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM16" si="9">AJ6-AL6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP16" si="10">AM6-AO6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS16" si="11">AP6-AR6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV16" si="12">AS6-AU6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY16" si="13">AV6-AX6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA16" si="15">G6-AZ6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2565,6 +2567,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2576,11 +2583,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CU generar recibo de pago terminado
Se termina la implementación del caso de uso generar recibo de pago, se actualizan las plantillas de la iteración
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F88AE7D5-81E9-486D-BA14-05C588728F8D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{203214C5-EF3A-4307-BEF6-6938D04C6A1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1070,90 +1070,92 @@
         <v>1</v>
       </c>
       <c r="M6" s="10"/>
-      <c r="N6" s="8"/>
+      <c r="N6" s="8">
+        <v>2</v>
+      </c>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O16" si="1">L6-N6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R16" si="2">O6-Q6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U16" si="3">R6-T6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X16" si="4">U6-W6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA16" si="5">X6-Z6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD16" si="6">AA6-AC6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG16" si="7">AD6-AF6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ16" si="8">AG6-AI6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM16" si="9">AJ6-AL6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP16" si="10">AM6-AO6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS16" si="11">AP6-AR6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV16" si="12">AS6-AU6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY16" si="13">AV6-AX6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA16" si="15">G6-AZ6</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2567,11 +2569,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2583,6 +2580,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Registro de pago temporal parcial
Se agrega interfaz grafica y logica/accesodatos parcial del registro
tempora de pagos para el director. Se actualizan modelos de datos y
plantilla de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{203214C5-EF3A-4307-BEF6-6938D04C6A1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3841E2F-2332-4A49-B293-36E04B6DE533}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1626,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G11" s="5">
         <v>2</v>
@@ -1649,84 +1649,86 @@
         <v>2</v>
       </c>
       <c r="P11" s="10"/>
-      <c r="Q11" s="8"/>
+      <c r="Q11" s="8">
+        <v>2</v>
+      </c>
       <c r="R11" s="8">
         <f>O11-Q11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S11" s="10"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8">
         <f>R11-T11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="8"/>
       <c r="X11" s="8">
         <f>U11-W11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8">
         <f>X11-Z11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB11" s="10"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="8">
         <f>AA11-AC11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE11" s="10"/>
       <c r="AF11" s="8"/>
       <c r="AG11" s="8">
         <f>AD11-AF11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="10"/>
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8">
         <f>AG11-AI11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK11" s="10"/>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8">
         <f>AJ11-AL11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN11" s="10"/>
       <c r="AO11" s="8"/>
       <c r="AP11" s="8">
         <f>AM11-AO11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="8">
         <f>AP11-AR11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT11" s="10"/>
       <c r="AU11" s="8"/>
       <c r="AV11" s="8">
         <f>AS11-AU11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW11" s="10"/>
       <c r="AX11" s="8"/>
       <c r="AY11" s="8">
         <f>AV11-AX11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ11" s="11">
         <f>H11+K11+N11+Q11+T11+W11+Z11+AC11+AF11+AI11+AL11+AO11+AR11+AU11+AX11</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA11" s="11">
         <f>G11-AZ11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:53" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2569,6 +2571,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2580,11 +2587,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Caso de uso reporte de ingresos y egresos parcial.
Se implementa parcialemente el caso de uso generar reporte de ingresos y egresos, se actualiza la plantilla de la iteracion
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3841E2F-2332-4A49-B293-36E04B6DE533}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1B2E83B7-BB3F-4DD1-9B8B-80130C062A8F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1285,7 @@
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
@@ -1302,90 +1302,92 @@
         <v>4</v>
       </c>
       <c r="M8" s="10"/>
-      <c r="N8" s="8"/>
+      <c r="N8" s="8">
+        <v>2</v>
+      </c>
       <c r="O8" s="8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2571,11 +2573,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2587,6 +2584,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implementacion del caso de uso generar reporte de ingresos y egresos parcial
Se implementa la segunda parte del caso de uso generar reporte de ingresos y egresos, se actualiza la plantilla de la iteración.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95067FC9-ACAB-47C9-BEAE-79CD3A999B3E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{357DEBFD-820C-415A-92B3-7CA8BC946359}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,78 +1316,80 @@
         <v>2</v>
       </c>
       <c r="S8" s="10"/>
-      <c r="T8" s="8"/>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2575,11 +2577,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2591,6 +2588,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementacion de caso de uso consultar ingresos y egresos
Tercera parte de la implementacion de caso de uso consultar ingresos y egresos, se actualiza la plantilla de la iteracion
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{357DEBFD-820C-415A-92B3-7CA8BC946359}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{194D29DB-30D5-4F34-9468-F035A5D13B10}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,90 +1189,92 @@
         <v>1</v>
       </c>
       <c r="M7" s="10"/>
-      <c r="N7" s="8"/>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2577,6 +2579,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2588,11 +2595,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementacion de caso de generar recibo de ingresos y egresos
cuarta iteracion de la implementacion del caso de uso generar recibo de ingresos y egresos, se actualiza la plantilla de la iteracion
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F32164-7575-4A2F-B6CF-7D372F0F3467}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E611C74-BC90-4B27-8B4A-B26860277CFF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,90 +1189,92 @@
         <v>1</v>
       </c>
       <c r="M7" s="10"/>
-      <c r="N7" s="8"/>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -1316,78 +1318,82 @@
         <v>2</v>
       </c>
       <c r="S8" s="10"/>
-      <c r="T8" s="8"/>
+      <c r="T8" s="8">
+        <v>1</v>
+      </c>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="V8" s="10"/>
+      <c r="W8" s="8">
         <v>2</v>
       </c>
-      <c r="V8" s="10"/>
-      <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -1628,7 +1634,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="5">
         <v>2</v>
@@ -2577,6 +2583,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2588,11 +2599,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementación del caso de uso consultar ingresos y egresos completado
Se implementa el caso de uso consultar ingresos y egresos (excluyendo las pruebas unitarias)... Se actualizan las plantillas de la iteración
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E611C74-BC90-4B27-8B4A-B26860277CFF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{83AB3F00-FDDF-4DBE-A821-4AA43906D840}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,7 +755,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,66 +1334,68 @@
         <v>-1</v>
       </c>
       <c r="Y8" s="10"/>
-      <c r="Z8" s="8"/>
+      <c r="Z8" s="8">
+        <v>4</v>
+      </c>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2583,11 +2585,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2599,6 +2596,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementacion del caso de uso  consultar registro de asistencias
se implementa el caso de consultar regitro de asistencias  de un grupo, se actualizan las plantillas de la iteracion y las tablas de pruebas
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 7ma Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82293E6-2F71-4521-91B9-EE1A6AFABF89}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{41F10401-BDD1-47A3-915E-93F3D46B7969}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>Columna</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>Mario</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
   <si>
     <t>CU Generar recibo de pago.</t>
@@ -752,7 +749,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,13 +1037,13 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1159,13 +1156,13 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G7" s="5">
         <v>4</v>
@@ -1280,13 +1277,13 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="5">
         <v>4</v>
@@ -1401,13 +1398,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G9" s="5">
         <v>3</v>
@@ -1516,13 +1513,13 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G10" s="5">
         <v>3</v>
@@ -1569,73 +1566,75 @@
         <v>4</v>
       </c>
       <c r="AB10" s="10"/>
-      <c r="AC10" s="8"/>
+      <c r="AC10" s="8">
+        <v>4</v>
+      </c>
       <c r="AD10" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK10" s="10"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AN10" s="10"/>
       <c r="AO10" s="8"/>
       <c r="AP10" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="8"/>
       <c r="AS10" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AT10" s="10"/>
       <c r="AU10" s="8"/>
       <c r="AV10" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AW10" s="10"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G11" s="5">
         <v>2</v>
@@ -2584,11 +2583,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2600,6 +2594,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>